<commit_message>
Ver 2.1 javascriptの圧縮 lazy loadの設定を追加
</commit_message>
<xml_diff>
--- a/style.xlsx
+++ b/style.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="32">
   <si>
     <t>#wordpress</t>
     <phoneticPr fontId="1"/>
@@ -118,17 +118,45 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>singular.php</t>
-  </si>
-  <si>
-    <t>index.php</t>
-  </si>
-  <si>
     <t>#content_text</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>.adsense</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>・</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>・</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>・</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>・</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>・</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>個別ページ</t>
+    <rPh sb="0" eb="2">
+      <t>コベツ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>月別、カテゴリー、アーカイブページ</t>
+    <rPh sb="0" eb="2">
+      <t>ツキベツ</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -303,7 +331,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -345,6 +373,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -662,8 +693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="U66" sqref="U66"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
@@ -673,7 +704,7 @@
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="5" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -1554,24 +1585,24 @@
       <c r="H29" s="6"/>
       <c r="I29" s="5"/>
       <c r="J29" s="4"/>
-      <c r="K29" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="L29" s="11"/>
-      <c r="M29" s="11"/>
-      <c r="N29" s="11"/>
-      <c r="O29" s="11"/>
-      <c r="P29" s="11"/>
-      <c r="Q29" s="11"/>
-      <c r="R29" s="11"/>
-      <c r="S29" s="11"/>
-      <c r="T29" s="11"/>
-      <c r="U29" s="11"/>
-      <c r="V29" s="11"/>
-      <c r="W29" s="11"/>
-      <c r="X29" s="11"/>
-      <c r="Y29" s="11"/>
-      <c r="Z29" s="12"/>
+      <c r="K29" s="5"/>
+      <c r="L29" s="5"/>
+      <c r="M29" s="5"/>
+      <c r="N29" s="5"/>
+      <c r="O29" s="5"/>
+      <c r="P29" s="5"/>
+      <c r="Q29" s="5"/>
+      <c r="R29" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="S29" s="5"/>
+      <c r="T29" s="5"/>
+      <c r="U29" s="5"/>
+      <c r="V29" s="5"/>
+      <c r="W29" s="5"/>
+      <c r="X29" s="5"/>
+      <c r="Y29" s="5"/>
+      <c r="Z29" s="5"/>
       <c r="AA29" s="6"/>
       <c r="AB29" s="13"/>
       <c r="AC29" s="6"/>
@@ -1594,7 +1625,9 @@
       <c r="O30" s="5"/>
       <c r="P30" s="5"/>
       <c r="Q30" s="5"/>
-      <c r="R30" s="5"/>
+      <c r="R30" s="14" t="s">
+        <v>28</v>
+      </c>
       <c r="S30" s="5"/>
       <c r="T30" s="5"/>
       <c r="U30" s="5"/>
@@ -1625,7 +1658,9 @@
       <c r="O31" s="5"/>
       <c r="P31" s="5"/>
       <c r="Q31" s="5"/>
-      <c r="R31" s="5"/>
+      <c r="R31" s="14" t="s">
+        <v>26</v>
+      </c>
       <c r="S31" s="5"/>
       <c r="T31" s="5"/>
       <c r="U31" s="5"/>
@@ -1656,7 +1691,9 @@
       <c r="O32" s="5"/>
       <c r="P32" s="5"/>
       <c r="Q32" s="5"/>
-      <c r="R32" s="5"/>
+      <c r="R32" s="14" t="s">
+        <v>29</v>
+      </c>
       <c r="S32" s="5"/>
       <c r="T32" s="5"/>
       <c r="U32" s="5"/>
@@ -1687,7 +1724,9 @@
       <c r="O33" s="5"/>
       <c r="P33" s="5"/>
       <c r="Q33" s="5"/>
-      <c r="R33" s="5"/>
+      <c r="R33" s="14" t="s">
+        <v>27</v>
+      </c>
       <c r="S33" s="5"/>
       <c r="T33" s="5"/>
       <c r="U33" s="5"/>
@@ -1718,7 +1757,9 @@
       <c r="O34" s="5"/>
       <c r="P34" s="5"/>
       <c r="Q34" s="5"/>
-      <c r="R34" s="5"/>
+      <c r="R34" s="14" t="s">
+        <v>25</v>
+      </c>
       <c r="S34" s="5"/>
       <c r="T34" s="5"/>
       <c r="U34" s="5"/>
@@ -1749,7 +1790,9 @@
       <c r="O35" s="5"/>
       <c r="P35" s="5"/>
       <c r="Q35" s="5"/>
-      <c r="R35" s="5"/>
+      <c r="R35" s="14" t="s">
+        <v>26</v>
+      </c>
       <c r="S35" s="5"/>
       <c r="T35" s="5"/>
       <c r="U35" s="5"/>
@@ -1780,7 +1823,6 @@
       <c r="O36" s="5"/>
       <c r="P36" s="5"/>
       <c r="Q36" s="5"/>
-      <c r="R36" s="5"/>
       <c r="S36" s="5"/>
       <c r="T36" s="5"/>
       <c r="U36" s="5"/>
@@ -1804,22 +1846,24 @@
       <c r="H37" s="6"/>
       <c r="I37" s="5"/>
       <c r="J37" s="4"/>
-      <c r="K37" s="5"/>
-      <c r="L37" s="5"/>
-      <c r="M37" s="5"/>
-      <c r="N37" s="5"/>
-      <c r="O37" s="5"/>
-      <c r="P37" s="5"/>
-      <c r="Q37" s="5"/>
-      <c r="R37" s="5"/>
-      <c r="S37" s="5"/>
-      <c r="T37" s="5"/>
-      <c r="U37" s="5"/>
-      <c r="V37" s="5"/>
-      <c r="W37" s="5"/>
-      <c r="X37" s="5"/>
-      <c r="Y37" s="5"/>
-      <c r="Z37" s="5"/>
+      <c r="K37" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="L37" s="11"/>
+      <c r="M37" s="11"/>
+      <c r="N37" s="11"/>
+      <c r="O37" s="11"/>
+      <c r="P37" s="11"/>
+      <c r="Q37" s="11"/>
+      <c r="R37" s="11"/>
+      <c r="S37" s="11"/>
+      <c r="T37" s="11"/>
+      <c r="U37" s="11"/>
+      <c r="V37" s="11"/>
+      <c r="W37" s="11"/>
+      <c r="X37" s="11"/>
+      <c r="Y37" s="11"/>
+      <c r="Z37" s="12"/>
       <c r="AA37" s="6"/>
       <c r="AB37" s="13"/>
       <c r="AC37" s="6"/>
@@ -1835,22 +1879,22 @@
       <c r="H38" s="6"/>
       <c r="I38" s="5"/>
       <c r="J38" s="4"/>
-      <c r="K38" s="5"/>
-      <c r="L38" s="5"/>
-      <c r="M38" s="5"/>
-      <c r="N38" s="5"/>
-      <c r="O38" s="5"/>
-      <c r="P38" s="5"/>
-      <c r="Q38" s="5"/>
-      <c r="R38" s="5"/>
-      <c r="S38" s="5"/>
-      <c r="T38" s="5"/>
-      <c r="U38" s="5"/>
-      <c r="V38" s="5"/>
-      <c r="W38" s="5"/>
-      <c r="X38" s="5"/>
-      <c r="Y38" s="5"/>
-      <c r="Z38" s="5"/>
+      <c r="K38" s="2"/>
+      <c r="L38" s="2"/>
+      <c r="M38" s="2"/>
+      <c r="N38" s="2"/>
+      <c r="O38" s="2"/>
+      <c r="P38" s="2"/>
+      <c r="Q38" s="2"/>
+      <c r="R38" s="2"/>
+      <c r="S38" s="2"/>
+      <c r="T38" s="2"/>
+      <c r="U38" s="2"/>
+      <c r="V38" s="2"/>
+      <c r="W38" s="2"/>
+      <c r="X38" s="2"/>
+      <c r="Y38" s="2"/>
+      <c r="Z38" s="2"/>
       <c r="AA38" s="6"/>
       <c r="AB38" s="13"/>
       <c r="AC38" s="6"/>
@@ -2014,7 +2058,7 @@
     </row>
     <row r="44" spans="1:29" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
     </row>
     <row r="45" spans="1:29" ht="9" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
@@ -2779,7 +2823,7 @@
       <c r="K69" s="4"/>
       <c r="L69" s="4"/>
       <c r="M69" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="N69" s="2"/>
       <c r="O69" s="2"/>
@@ -2844,7 +2888,7 @@
       <c r="L71" s="4"/>
       <c r="M71" s="4"/>
       <c r="N71" s="10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="O71" s="11"/>
       <c r="P71" s="11"/>

</xml_diff>